<commit_message>
Add features to display bid data in admin dashboard
</commit_message>
<xml_diff>
--- a/bids.xlsx
+++ b/bids.xlsx
@@ -397,69 +397,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Bid</v>
+      </c>
+      <c r="B1" t="str">
+        <v>College</v>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>indrajit</v>
+      <c r="A2">
+        <v>89</v>
       </c>
       <c r="B2" t="str">
-        <v>indrajit.chandra.MBA23@said.oxford.edu</v>
-      </c>
-      <c r="C2">
-        <v>67</v>
+        <v>oxford university</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>indrajit chandra</v>
+        <v>indrajit</v>
       </c>
       <c r="B3" t="str">
         <v>indrajit.chandra.MBA23@said.oxford.edu</v>
       </c>
-      <c r="C3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>pritam chabra</v>
-      </c>
-      <c r="B4" t="str">
-        <v>pritam.chabra.MBA23@said.oxford.edu</v>
-      </c>
-      <c r="C4">
+      <c r="C3" t="str">
+        <v>9732253783</v>
+      </c>
+      <c r="D3">
         <v>89</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>pritam chabra</v>
-      </c>
-      <c r="B5" t="str">
-        <v>pritam.chabra.MBA23@said.oxford.edu</v>
-      </c>
-      <c r="C5">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>subham</v>
-      </c>
-      <c r="B6" t="str">
-        <v>subham.saha.MBA23@said.oxford.edu</v>
-      </c>
-      <c r="C6">
-        <v>321</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>